<commit_message>
Fixed a bug with statsmodels and add 3 more charts
</commit_message>
<xml_diff>
--- a/Mash3_BGS_Talk_v02b.xlsx
+++ b/Mash3_BGS_Talk_v02b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\Matias\Proyectos personales\Mash3_simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD03340-CDBF-4FFF-A487-9F18D1617AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9AE22C-79DB-4B93-A03E-9747EF3A3D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>

</xml_diff>